<commit_message>
add new login test worksheet
</commit_message>
<xml_diff>
--- a/SauceLabAutomationWithParralletTesting/src/test/resources/LoginMaterial.xlsx
+++ b/SauceLabAutomationWithParralletTesting/src/test/resources/LoginMaterial.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\eclipse-workspace\SauceLabAutomationWithParralletTesting\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\ParallelTest\SauceLabAutomationWithParralletTesting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C31B63-D8DE-40DE-92A7-317744025C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C53397-F255-426E-BDDC-9B799B9B81C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0E83CD2E-CCF1-425F-9152-7D58BA3CE6A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{0E83CD2E-CCF1-425F-9152-7D58BA3CE6A7}"/>
   </bookViews>
   <sheets>
     <sheet name="sauceLoginTest" sheetId="3" r:id="rId1"/>
-    <sheet name="InformationPageTest" sheetId="4" r:id="rId2"/>
+    <sheet name="sauceLoginsTest" sheetId="5" r:id="rId2"/>
+    <sheet name="InformationPageTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Password</t>
   </si>
@@ -53,6 +54,15 @@
   </si>
   <si>
     <t>Oscar</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -407,7 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D0863F-D4E0-4041-9C6A-5942347310B8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -437,6 +447,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637FCB99-667C-40F4-A6C0-896062A7A4CE}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3926EB-54CD-4FC4-A654-E96CEFE26D1F}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
change in test method
</commit_message>
<xml_diff>
--- a/SauceLabAutomationWithParralletTesting/src/test/resources/LoginMaterial.xlsx
+++ b/SauceLabAutomationWithParralletTesting/src/test/resources/LoginMaterial.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\ParallelTest\SauceLabAutomationWithParralletTesting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86777743-1F91-474D-BECF-0BBDB47B34FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C622A042-AA29-4DD6-B612-F4AFE6BB2B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{0E83CD2E-CCF1-425F-9152-7D58BA3CE6A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{0E83CD2E-CCF1-425F-9152-7D58BA3CE6A7}"/>
   </bookViews>
   <sheets>
     <sheet name="sauceLoginTest" sheetId="3" r:id="rId1"/>
-    <sheet name="sauceLoginsTest" sheetId="5" r:id="rId2"/>
-    <sheet name="InformationPageTest" sheetId="4" r:id="rId3"/>
+    <sheet name="InformationPageTest" sheetId="4" r:id="rId2"/>
+    <sheet name="sauceLoginsTest" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Password</t>
   </si>
@@ -63,16 +63,32 @@
   </si>
   <si>
     <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +464,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637FCB99-667C-40F4-A6C0-896062A7A4CE}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3926EB-54CD-4FC4-A654-E96CEFE26D1F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738B9796-3AF2-432C-95DA-C7317A27AE4F}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,78 +511,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3926EB-54CD-4FC4-A654-E96CEFE26D1F}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1">
-        <v>10123</v>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>